<commit_message>
Update Month/Quarter with 2019, Personal Income
</commit_message>
<xml_diff>
--- a/CleanedData/MonthQuarter.xlsx
+++ b/CleanedData/MonthQuarter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalievallejo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalievallejo/Desktop/Final Project CSVs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{852C965D-B864-3940-931D-139446F6E390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C4871B-D279-3648-9790-63E29DB41DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="500" windowWidth="27060" windowHeight="16940" xr2:uid="{87633D09-E304-E24B-94DC-CBB28599983A}"/>
+    <workbookView xWindow="11920" yWindow="500" windowWidth="27060" windowHeight="16940" xr2:uid="{87633D09-E304-E24B-94DC-CBB28599983A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>Month</t>
   </si>
@@ -78,13 +78,25 @@
   </si>
   <si>
     <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2019Q1</t>
+  </si>
+  <si>
+    <t>2019Q2</t>
+  </si>
+  <si>
+    <t>2019Q3</t>
+  </si>
+  <si>
+    <t>2019Q4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +108,12 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E511CA-DF83-E449-942D-407583C2B905}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,279 +478,384 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>43831</v>
+        <v>43466</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43862</v>
+        <v>43497</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>43922</v>
+        <v>43525</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>43952</v>
+        <v>43556</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>43983</v>
+        <v>43586</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44013</v>
+        <v>43617</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44044</v>
+        <v>43647</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44075</v>
+        <v>43678</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44105</v>
+        <v>43709</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44136</v>
+        <v>43739</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44166</v>
+        <v>43770</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44197</v>
+        <v>43800</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44228</v>
+        <v>43831</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44256</v>
+        <v>43862</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44287</v>
+        <v>43891</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44317</v>
+        <v>43922</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44348</v>
+        <v>43952</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44378</v>
+        <v>43983</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44409</v>
+        <v>44013</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44440</v>
+        <v>44044</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44470</v>
+        <v>44075</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44501</v>
+        <v>44105</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44531</v>
+        <v>44136</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44562</v>
+        <v>44166</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44593</v>
+        <v>44197</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44621</v>
+        <v>44228</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44652</v>
+        <v>44256</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44682</v>
+        <v>44287</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44713</v>
+        <v>44317</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44743</v>
+        <v>44348</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44774</v>
+        <v>44378</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44805</v>
+        <v>44409</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44835</v>
+        <v>44440</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
+        <v>44470</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>44501</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>44531</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>44562</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>44593</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>44621</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>44652</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>44682</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>44713</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>44743</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>44805</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>44866</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>